<commit_message>
add utility resources with maps and examples
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.immunization.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.immunization.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-12-23T08:33:50-06:00</t>
+    <t>2022-12-23T15:55:29-06:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -268,7 +268,7 @@
     <t>Mapping: CDA (R2)</t>
   </si>
   <si>
-    <t>Mapping: VIA/VDIF to MHV-PHR</t>
+    <t>Mapping: VDIF to MHV-PHR</t>
   </si>
   <si>
     <t/>

</xml_diff>

<commit_message>
add more notes, and add labs
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.immunization.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.immunization.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-12-23T15:55:29-06:00</t>
+    <t>2023-01-04T18:59:45-06:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -92,7 +92,7 @@
 * must have status of completed 
 * must have identifier as cross reference to original source
 * must have a code.text or code.coding from a valueset
-  * code.coding may should be a CVX but we don't have such.
+  * code.coding should be a CVX but we don't have such.
   * Might have a CPT code
 * must have a date (occuranceDateTime) the vaccine was administered from the UI
   * will also be used for recorded date
@@ -100,7 +100,16 @@
 * any reaction is recorded as a contained observation
 * may have a comment note
 * once created will have an id, versionId, lastUpdated.
-* Not sure if text will be populated</t>
+* Not sure if text will be populated
+Mapping from [ImmunizationTO](StructureDefinition-VA.MHV.PHR.immunization-mappings.html#mappings-for-vdif-to-mhv-phr-immunizationto)
+TODO Questions: 
+- The given mock example aligns with both VIA_v4.0.7_uat.wsdl and mockey-mdws3-service.wsdl. The VIA schema has more elements. The mapping is only for elements that were in both and for which I had an example. Better mapping can be done if specific schema can be identifed, and more rich mock example.
+- reaction appears to be a controlled vocabulary (e.g. FEVER), or is it a number (1-11 - convertReactionCode())?
+- contraindicated -- appears to be a number (e.g. 0). No idea what the values might be or what they might mean
+- id - presuming this is a persisted identifier we can cross-reference with
+- series - this appears to be a controlled vocabulary (e.g. COMPLETE). What are the possible values and what do they mean?
+- encounter - should we convert these to instances of FHIR Encounter?
+- could have function that converts a defined set of ImmunizationTO.name values to proper codes. This might be an advanced feature.</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -1198,7 +1207,7 @@
     <t>Immunization.site.text</t>
   </si>
   <si>
-    <t>ImmunizationTO.anatomicSurvace</t>
+    <t>ImmunizationTO.anatomicSurface</t>
   </si>
   <si>
     <t>Immunization.route</t>

</xml_diff>

<commit_message>
updates for Identifier management
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.immunization.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.immunization.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4035" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4035" uniqueCount="629">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-02-23T08:47:22-06:00</t>
+    <t>2023-03-05T12:38:40-06:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -530,7 +530,7 @@
     <t>ClinicalDocument/component/StructuredBody/component/section/entry/substanceAdministration/id</t>
   </si>
   <si>
-    <t>ImmunizationTO.id</t>
+    <t>{StationNbr} | `;` | {ImmunizationTO.id}</t>
   </si>
   <si>
     <t>Immunization.identifier:TOid</t>
@@ -659,7 +659,7 @@
     <t>Immunization.identifier.system</t>
   </si>
   <si>
-    <t>system for given Vista site and ImmunizationTO.id</t>
+    <t>The namespace for the identifier value</t>
   </si>
   <si>
     <t>Establishes the namespace for the value - that is, a URL that describes a set values that are unique.</t>
@@ -669,6 +669,9 @@
   </si>
   <si>
     <t>There are many sets  of identifiers.  To perform matching of two identifiers, we need to know what set we're dealing with. The system identifies a particular set of unique identifiers.</t>
+  </si>
+  <si>
+    <t>urn:oid:2.16.840.1.113883.4.349</t>
   </si>
   <si>
     <t>http://www.acme.com/identifiers/patient</t>
@@ -4328,10 +4331,10 @@
         <v>79</v>
       </c>
       <c r="S17" t="s" s="2">
-        <v>79</v>
+        <v>203</v>
       </c>
       <c r="T17" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="U17" t="s" s="2">
         <v>79</v>
@@ -4367,7 +4370,7 @@
         <v>79</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>80</v>
@@ -4385,10 +4388,10 @@
         <v>79</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AN17" t="s" s="2">
         <v>79</v>
@@ -4402,10 +4405,10 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -4434,10 +4437,10 @@
         <v>157</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="O18" s="2"/>
       <c r="P18" t="s" s="2">
@@ -4451,7 +4454,7 @@
         <v>79</v>
       </c>
       <c r="T18" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="U18" t="s" s="2">
         <v>79</v>
@@ -4487,7 +4490,7 @@
         <v>79</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>80</v>
@@ -4505,10 +4508,10 @@
         <v>79</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="AN18" t="s" s="2">
         <v>79</v>
@@ -4522,10 +4525,10 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -4548,13 +4551,13 @@
         <v>91</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
@@ -4605,7 +4608,7 @@
         <v>79</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>80</v>
@@ -4623,10 +4626,10 @@
         <v>79</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="AN19" t="s" s="2">
         <v>79</v>
@@ -4640,10 +4643,10 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
@@ -4666,16 +4669,16 @@
         <v>91</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="O20" s="2"/>
       <c r="P20" t="s" s="2">
@@ -4725,7 +4728,7 @@
         <v>79</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>80</v>
@@ -4743,10 +4746,10 @@
         <v>79</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="AN20" t="s" s="2">
         <v>79</v>
@@ -4760,10 +4763,10 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -4789,13 +4792,13 @@
         <v>110</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="O21" s="2"/>
       <c r="P21" t="s" s="2">
@@ -4806,7 +4809,7 @@
         <v>79</v>
       </c>
       <c r="S21" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="T21" t="s" s="2">
         <v>79</v>
@@ -4825,7 +4828,7 @@
       </c>
       <c r="Y21" s="2"/>
       <c r="Z21" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AA21" t="s" s="2">
         <v>79</v>
@@ -4843,7 +4846,7 @@
         <v>79</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>90</v>
@@ -4858,30 +4861,30 @@
         <v>102</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="AL21" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AP21" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -4907,13 +4910,13 @@
         <v>187</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="O22" s="2"/>
       <c r="P22" t="s" s="2">
@@ -4939,11 +4942,11 @@
         <v>79</v>
       </c>
       <c r="X22" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Y22" s="2"/>
       <c r="Z22" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AA22" t="s" s="2">
         <v>79</v>
@@ -4961,7 +4964,7 @@
         <v>79</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>80</v>
@@ -4976,13 +4979,13 @@
         <v>102</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AL22" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN22" t="s" s="2">
         <v>79</v>
@@ -4996,10 +4999,10 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -5025,10 +5028,10 @@
         <v>187</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -5059,7 +5062,7 @@
       </c>
       <c r="Y23" s="2"/>
       <c r="Z23" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AA23" t="s" s="2">
         <v>79</v>
@@ -5077,7 +5080,7 @@
         <v>79</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>90</v>
@@ -5086,25 +5089,25 @@
         <v>90</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AJ23" t="s" s="2">
         <v>102</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AO23" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AP23" t="s" s="2">
         <v>79</v>
@@ -5112,10 +5115,10 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -5230,10 +5233,10 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -5350,10 +5353,10 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -5376,19 +5379,19 @@
         <v>91</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O26" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="P26" t="s" s="2">
         <v>79</v>
@@ -5437,7 +5440,7 @@
         <v>79</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>80</v>
@@ -5455,10 +5458,10 @@
         <v>79</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>79</v>
@@ -5472,10 +5475,10 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -5590,10 +5593,10 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -5710,10 +5713,10 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -5739,16 +5742,16 @@
         <v>104</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="N29" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="O29" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="P29" t="s" s="2">
         <v>79</v>
@@ -5797,7 +5800,7 @@
         <v>79</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>80</v>
@@ -5815,10 +5818,10 @@
         <v>79</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>79</v>
@@ -5832,10 +5835,10 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -5861,13 +5864,13 @@
         <v>162</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" t="s" s="2">
@@ -5917,7 +5920,7 @@
         <v>79</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>80</v>
@@ -5935,10 +5938,10 @@
         <v>79</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>79</v>
@@ -5952,10 +5955,10 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5981,14 +5984,14 @@
         <v>110</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="P31" t="s" s="2">
         <v>79</v>
@@ -6037,7 +6040,7 @@
         <v>79</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>80</v>
@@ -6055,10 +6058,10 @@
         <v>79</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>79</v>
@@ -6067,15 +6070,15 @@
         <v>79</v>
       </c>
       <c r="AP31" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -6101,14 +6104,14 @@
         <v>162</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="P32" t="s" s="2">
         <v>79</v>
@@ -6157,7 +6160,7 @@
         <v>79</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>80</v>
@@ -6175,10 +6178,10 @@
         <v>79</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>79</v>
@@ -6187,15 +6190,15 @@
         <v>79</v>
       </c>
       <c r="AP32" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -6218,19 +6221,19 @@
         <v>91</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="O33" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="P33" t="s" s="2">
         <v>79</v>
@@ -6279,7 +6282,7 @@
         <v>79</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>80</v>
@@ -6297,10 +6300,10 @@
         <v>79</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>79</v>
@@ -6314,10 +6317,10 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -6343,16 +6346,16 @@
         <v>162</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="N34" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="O34" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="P34" t="s" s="2">
         <v>79</v>
@@ -6401,7 +6404,7 @@
         <v>79</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>80</v>
@@ -6419,10 +6422,10 @@
         <v>79</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>79</v>
@@ -6431,19 +6434,19 @@
         <v>79</v>
       </c>
       <c r="AP34" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" t="s" s="2">
@@ -6462,13 +6465,13 @@
         <v>91</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
@@ -6519,7 +6522,7 @@
         <v>79</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>90</v>
@@ -6534,30 +6537,30 @@
         <v>102</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AN35" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="AO35" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AP35" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -6580,13 +6583,13 @@
         <v>79</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -6637,7 +6640,7 @@
         <v>79</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>80</v>
@@ -6652,30 +6655,30 @@
         <v>102</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="AN36" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="AO36" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AP36" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -6698,16 +6701,16 @@
         <v>91</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="O37" s="2"/>
       <c r="P37" t="s" s="2">
@@ -6745,17 +6748,17 @@
         <v>79</v>
       </c>
       <c r="AB37" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>90</v>
@@ -6770,19 +6773,19 @@
         <v>102</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="AN37" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="AO37" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AP37" t="s" s="2">
         <v>79</v>
@@ -6790,13 +6793,13 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C38" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D38" t="s" s="2">
         <v>79</v>
@@ -6818,16 +6821,16 @@
         <v>91</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="O38" s="2"/>
       <c r="P38" t="s" s="2">
@@ -6877,7 +6880,7 @@
         <v>79</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>90</v>
@@ -6892,30 +6895,30 @@
         <v>102</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="AO38" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AP38" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -6938,13 +6941,13 @@
         <v>79</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -6995,7 +6998,7 @@
         <v>79</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>80</v>
@@ -7016,24 +7019,24 @@
         <v>79</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AN39" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="AO39" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AP39" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -7056,16 +7059,16 @@
         <v>91</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="O40" s="2"/>
       <c r="P40" t="s" s="2">
@@ -7115,7 +7118,7 @@
         <v>79</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>80</v>
@@ -7133,27 +7136,27 @@
         <v>79</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AN40" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AO40" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AP40" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -7179,13 +7182,13 @@
         <v>187</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="O41" s="2"/>
       <c r="P41" t="s" s="2">
@@ -7211,13 +7214,13 @@
         <v>79</v>
       </c>
       <c r="X41" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Y41" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="Z41" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="AA41" t="s" s="2">
         <v>79</v>
@@ -7235,7 +7238,7 @@
         <v>79</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>80</v>
@@ -7253,13 +7256,13 @@
         <v>79</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AN41" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AO41" t="s" s="2">
         <v>79</v>
@@ -7270,10 +7273,10 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -7296,13 +7299,13 @@
         <v>79</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
@@ -7353,7 +7356,7 @@
         <v>79</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>80</v>
@@ -7368,16 +7371,16 @@
         <v>102</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="AN42" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="AO42" t="s" s="2">
         <v>79</v>
@@ -7388,10 +7391,10 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -7506,10 +7509,10 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -7626,10 +7629,10 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -7655,13 +7658,13 @@
         <v>162</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="N45" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="O45" s="2"/>
       <c r="P45" t="s" s="2">
@@ -7711,7 +7714,7 @@
         <v>79</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>80</v>
@@ -7720,7 +7723,7 @@
         <v>90</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="AJ45" t="s" s="2">
         <v>102</v>
@@ -7746,10 +7749,10 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -7775,13 +7778,13 @@
         <v>104</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="N46" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="O46" s="2"/>
       <c r="P46" t="s" s="2">
@@ -7810,10 +7813,10 @@
         <v>192</v>
       </c>
       <c r="Y46" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="Z46" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="AA46" t="s" s="2">
         <v>79</v>
@@ -7831,7 +7834,7 @@
         <v>79</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>80</v>
@@ -7866,10 +7869,10 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -7895,13 +7898,13 @@
         <v>148</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="O47" s="2"/>
       <c r="P47" t="s" s="2">
@@ -7951,7 +7954,7 @@
         <v>79</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>80</v>
@@ -7972,7 +7975,7 @@
         <v>79</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>79</v>
@@ -7986,10 +7989,10 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -8015,13 +8018,13 @@
         <v>162</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="O48" s="2"/>
       <c r="P48" t="s" s="2">
@@ -8071,7 +8074,7 @@
         <v>79</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>80</v>
@@ -8101,15 +8104,15 @@
         <v>79</v>
       </c>
       <c r="AP48" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -8132,13 +8135,13 @@
         <v>79</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -8189,7 +8192,7 @@
         <v>79</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>80</v>
@@ -8207,27 +8210,27 @@
         <v>79</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AO49" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="AP49" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -8253,10 +8256,10 @@
         <v>162</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
@@ -8307,7 +8310,7 @@
         <v>79</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>80</v>
@@ -8325,27 +8328,27 @@
         <v>79</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AO50" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AP50" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -8368,13 +8371,13 @@
         <v>79</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
@@ -8425,7 +8428,7 @@
         <v>79</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>80</v>
@@ -8443,10 +8446,10 @@
         <v>79</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>79</v>
@@ -8460,10 +8463,10 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -8489,10 +8492,10 @@
         <v>187</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
@@ -8519,13 +8522,13 @@
         <v>79</v>
       </c>
       <c r="X52" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Y52" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="Z52" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="AA52" t="s" s="2">
         <v>79</v>
@@ -8543,7 +8546,7 @@
         <v>79</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>80</v>
@@ -8561,16 +8564,16 @@
         <v>79</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AO52" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="AP52" t="s" s="2">
         <v>79</v>
@@ -8578,10 +8581,10 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -8696,10 +8699,10 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -8816,10 +8819,10 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
@@ -8842,19 +8845,19 @@
         <v>91</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N55" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O55" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="P55" t="s" s="2">
         <v>79</v>
@@ -8903,7 +8906,7 @@
         <v>79</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>80</v>
@@ -8921,10 +8924,10 @@
         <v>79</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="AN55" t="s" s="2">
         <v>79</v>
@@ -8938,10 +8941,10 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
@@ -8967,16 +8970,16 @@
         <v>162</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="N56" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="O56" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="P56" t="s" s="2">
         <v>79</v>
@@ -9025,7 +9028,7 @@
         <v>79</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>80</v>
@@ -9043,10 +9046,10 @@
         <v>79</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="AN56" t="s" s="2">
         <v>79</v>
@@ -9055,15 +9058,15 @@
         <v>79</v>
       </c>
       <c r="AP56" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
@@ -9089,10 +9092,10 @@
         <v>187</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="N57" s="2"/>
       <c r="O57" s="2"/>
@@ -9119,13 +9122,13 @@
         <v>79</v>
       </c>
       <c r="X57" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Y57" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="Z57" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AA57" t="s" s="2">
         <v>79</v>
@@ -9143,7 +9146,7 @@
         <v>79</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>80</v>
@@ -9161,16 +9164,16 @@
         <v>79</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AN57" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AO57" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AP57" t="s" s="2">
         <v>79</v>
@@ -9178,10 +9181,10 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
@@ -9204,13 +9207,13 @@
         <v>79</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
@@ -9261,7 +9264,7 @@
         <v>79</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>80</v>
@@ -9279,10 +9282,10 @@
         <v>79</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="AN58" t="s" s="2">
         <v>79</v>
@@ -9296,10 +9299,10 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -9322,13 +9325,13 @@
         <v>91</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
@@ -9379,7 +9382,7 @@
         <v>79</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>80</v>
@@ -9394,13 +9397,13 @@
         <v>102</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="AN59" t="s" s="2">
         <v>79</v>
@@ -9414,10 +9417,10 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -9532,10 +9535,10 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -9652,14 +9655,14 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" t="s" s="2">
@@ -9681,10 +9684,10 @@
         <v>136</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="N62" t="s" s="2">
         <v>139</v>
@@ -9739,7 +9742,7 @@
         <v>79</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>80</v>
@@ -9774,10 +9777,10 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
@@ -9803,10 +9806,10 @@
         <v>187</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" s="2"/>
@@ -9836,10 +9839,10 @@
         <v>192</v>
       </c>
       <c r="Y63" t="s" s="2">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="Z63" t="s" s="2">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="AA63" t="s" s="2">
         <v>79</v>
@@ -9857,7 +9860,7 @@
         <v>79</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>80</v>
@@ -9872,13 +9875,13 @@
         <v>102</v>
       </c>
       <c r="AK63" t="s" s="2">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AL63" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AM63" t="s" s="2">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="AN63" t="s" s="2">
         <v>79</v>
@@ -9892,10 +9895,10 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
@@ -9918,16 +9921,16 @@
         <v>91</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="N64" t="s" s="2">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="O64" s="2"/>
       <c r="P64" t="s" s="2">
@@ -9977,7 +9980,7 @@
         <v>79</v>
       </c>
       <c r="AF64" t="s" s="2">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="AG64" t="s" s="2">
         <v>90</v>
@@ -9992,16 +9995,16 @@
         <v>102</v>
       </c>
       <c r="AK64" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="AL64" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AM64" t="s" s="2">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="AN64" t="s" s="2">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="AO64" t="s" s="2">
         <v>79</v>
@@ -10012,10 +10015,10 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" t="s" s="2">
@@ -10130,10 +10133,10 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
@@ -10250,10 +10253,10 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" t="s" s="2">
@@ -10279,13 +10282,13 @@
         <v>162</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="N67" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="O67" s="2"/>
       <c r="P67" t="s" s="2">
@@ -10335,7 +10338,7 @@
         <v>79</v>
       </c>
       <c r="AF67" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="AG67" t="s" s="2">
         <v>80</v>
@@ -10344,7 +10347,7 @@
         <v>90</v>
       </c>
       <c r="AI67" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="AJ67" t="s" s="2">
         <v>102</v>
@@ -10370,10 +10373,10 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B68" t="s" s="2">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" t="s" s="2">
@@ -10399,13 +10402,13 @@
         <v>104</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="M68" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="N68" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="O68" s="2"/>
       <c r="P68" t="s" s="2">
@@ -10434,10 +10437,10 @@
         <v>192</v>
       </c>
       <c r="Y68" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="Z68" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="AA68" t="s" s="2">
         <v>79</v>
@@ -10455,7 +10458,7 @@
         <v>79</v>
       </c>
       <c r="AF68" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="AG68" t="s" s="2">
         <v>80</v>
@@ -10490,10 +10493,10 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B69" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" t="s" s="2">
@@ -10519,13 +10522,13 @@
         <v>148</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="M69" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="N69" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="O69" s="2"/>
       <c r="P69" t="s" s="2">
@@ -10575,7 +10578,7 @@
         <v>79</v>
       </c>
       <c r="AF69" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="AG69" t="s" s="2">
         <v>80</v>
@@ -10596,7 +10599,7 @@
         <v>79</v>
       </c>
       <c r="AM69" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AN69" t="s" s="2">
         <v>79</v>
@@ -10610,10 +10613,10 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" t="s" s="2">
@@ -10639,13 +10642,13 @@
         <v>162</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="M70" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="N70" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="O70" s="2"/>
       <c r="P70" t="s" s="2">
@@ -10695,7 +10698,7 @@
         <v>79</v>
       </c>
       <c r="AF70" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="AG70" t="s" s="2">
         <v>80</v>
@@ -10725,15 +10728,15 @@
         <v>79</v>
       </c>
       <c r="AP70" t="s" s="2">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" t="s" s="2">
@@ -10756,13 +10759,13 @@
         <v>91</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="M71" t="s" s="2">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="N71" s="2"/>
       <c r="O71" s="2"/>
@@ -10813,7 +10816,7 @@
         <v>79</v>
       </c>
       <c r="AF71" t="s" s="2">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="AG71" t="s" s="2">
         <v>80</v>
@@ -10828,13 +10831,13 @@
         <v>102</v>
       </c>
       <c r="AK71" t="s" s="2">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="AL71" t="s" s="2">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="AM71" t="s" s="2">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="AN71" t="s" s="2">
         <v>79</v>
@@ -10848,10 +10851,10 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" t="s" s="2">
@@ -10966,10 +10969,10 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" t="s" s="2">
@@ -11086,10 +11089,10 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s" s="2">
@@ -11112,16 +11115,16 @@
         <v>91</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="M74" t="s" s="2">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="N74" t="s" s="2">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="O74" s="2"/>
       <c r="P74" t="s" s="2">
@@ -11171,7 +11174,7 @@
         <v>79</v>
       </c>
       <c r="AF74" t="s" s="2">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="AG74" t="s" s="2">
         <v>80</v>
@@ -11192,7 +11195,7 @@
         <v>133</v>
       </c>
       <c r="AM74" t="s" s="2">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="AN74" t="s" s="2">
         <v>79</v>
@@ -11206,10 +11209,10 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B75" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" t="s" s="2">
@@ -11232,13 +11235,13 @@
         <v>91</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="M75" t="s" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="N75" s="2"/>
       <c r="O75" s="2"/>
@@ -11289,7 +11292,7 @@
         <v>79</v>
       </c>
       <c r="AF75" t="s" s="2">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="AG75" t="s" s="2">
         <v>80</v>
@@ -11310,7 +11313,7 @@
         <v>133</v>
       </c>
       <c r="AM75" t="s" s="2">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="AN75" t="s" s="2">
         <v>79</v>
@@ -11324,10 +11327,10 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B76" t="s" s="2">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" t="s" s="2">
@@ -11350,13 +11353,13 @@
         <v>91</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="M76" t="s" s="2">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="N76" s="2"/>
       <c r="O76" s="2"/>
@@ -11407,7 +11410,7 @@
         <v>79</v>
       </c>
       <c r="AF76" t="s" s="2">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="AG76" t="s" s="2">
         <v>90</v>
@@ -11428,7 +11431,7 @@
         <v>133</v>
       </c>
       <c r="AM76" t="s" s="2">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="AN76" t="s" s="2">
         <v>79</v>
@@ -11437,15 +11440,15 @@
         <v>79</v>
       </c>
       <c r="AP76" t="s" s="2">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B77" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" t="s" s="2">
@@ -11471,10 +11474,10 @@
         <v>187</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="M77" t="s" s="2">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="N77" s="2"/>
       <c r="O77" s="2"/>
@@ -11501,13 +11504,13 @@
         <v>79</v>
       </c>
       <c r="X77" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Y77" t="s" s="2">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="Z77" t="s" s="2">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="AA77" t="s" s="2">
         <v>79</v>
@@ -11525,7 +11528,7 @@
         <v>79</v>
       </c>
       <c r="AF77" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="AG77" t="s" s="2">
         <v>80</v>
@@ -11540,13 +11543,13 @@
         <v>102</v>
       </c>
       <c r="AK77" t="s" s="2">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="AL77" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AM77" t="s" s="2">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="AN77" t="s" s="2">
         <v>79</v>
@@ -11560,10 +11563,10 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B78" t="s" s="2">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" t="s" s="2">
@@ -11586,13 +11589,13 @@
         <v>79</v>
       </c>
       <c r="K78" t="s" s="2">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="M78" t="s" s="2">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="N78" s="2"/>
       <c r="O78" s="2"/>
@@ -11643,7 +11646,7 @@
         <v>79</v>
       </c>
       <c r="AF78" t="s" s="2">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="AG78" t="s" s="2">
         <v>80</v>
@@ -11658,7 +11661,7 @@
         <v>102</v>
       </c>
       <c r="AK78" t="s" s="2">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="AL78" t="s" s="2">
         <v>79</v>
@@ -11678,10 +11681,10 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B79" t="s" s="2">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" t="s" s="2">
@@ -11704,23 +11707,23 @@
         <v>91</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="M79" t="s" s="2">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="N79" t="s" s="2">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="O79" s="2"/>
       <c r="P79" t="s" s="2">
         <v>79</v>
       </c>
       <c r="Q79" t="s" s="2">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="R79" t="s" s="2">
         <v>79</v>
@@ -11765,7 +11768,7 @@
         <v>79</v>
       </c>
       <c r="AF79" t="s" s="2">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="AG79" t="s" s="2">
         <v>80</v>
@@ -11783,7 +11786,7 @@
         <v>79</v>
       </c>
       <c r="AL79" t="s" s="2">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="AM79" t="s" s="2">
         <v>133</v>
@@ -11800,10 +11803,10 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B80" t="s" s="2">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" t="s" s="2">
@@ -11829,10 +11832,10 @@
         <v>187</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="M80" t="s" s="2">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="N80" s="2"/>
       <c r="O80" s="2"/>
@@ -11859,13 +11862,13 @@
         <v>79</v>
       </c>
       <c r="X80" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Y80" t="s" s="2">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="Z80" t="s" s="2">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="AA80" t="s" s="2">
         <v>79</v>
@@ -11883,7 +11886,7 @@
         <v>79</v>
       </c>
       <c r="AF80" t="s" s="2">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="AG80" t="s" s="2">
         <v>80</v>
@@ -11918,10 +11921,10 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B81" t="s" s="2">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" t="s" s="2">
@@ -11944,13 +11947,13 @@
         <v>79</v>
       </c>
       <c r="K81" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="M81" t="s" s="2">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="N81" s="2"/>
       <c r="O81" s="2"/>
@@ -12001,7 +12004,7 @@
         <v>79</v>
       </c>
       <c r="AF81" t="s" s="2">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="AG81" t="s" s="2">
         <v>80</v>
@@ -12013,7 +12016,7 @@
         <v>79</v>
       </c>
       <c r="AJ81" t="s" s="2">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="AK81" t="s" s="2">
         <v>79</v>
@@ -12036,10 +12039,10 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B82" t="s" s="2">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" t="s" s="2">
@@ -12154,10 +12157,10 @@
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B83" t="s" s="2">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" t="s" s="2">
@@ -12274,14 +12277,14 @@
     </row>
     <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B84" t="s" s="2">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="E84" s="2"/>
       <c r="F84" t="s" s="2">
@@ -12303,10 +12306,10 @@
         <v>136</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="M84" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="N84" t="s" s="2">
         <v>139</v>
@@ -12361,7 +12364,7 @@
         <v>79</v>
       </c>
       <c r="AF84" t="s" s="2">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="AG84" t="s" s="2">
         <v>80</v>
@@ -12396,10 +12399,10 @@
     </row>
     <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="B85" t="s" s="2">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" t="s" s="2">
@@ -12425,10 +12428,10 @@
         <v>162</v>
       </c>
       <c r="L85" t="s" s="2">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="M85" t="s" s="2">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="N85" s="2"/>
       <c r="O85" s="2"/>
@@ -12479,7 +12482,7 @@
         <v>79</v>
       </c>
       <c r="AF85" t="s" s="2">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="AG85" t="s" s="2">
         <v>80</v>
@@ -12497,7 +12500,7 @@
         <v>79</v>
       </c>
       <c r="AL85" t="s" s="2">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="AM85" t="s" s="2">
         <v>133</v>
@@ -12514,10 +12517,10 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B86" t="s" s="2">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" t="s" s="2">
@@ -12543,10 +12546,10 @@
         <v>104</v>
       </c>
       <c r="L86" t="s" s="2">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="M86" t="s" s="2">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="N86" s="2"/>
       <c r="O86" s="2"/>
@@ -12597,7 +12600,7 @@
         <v>79</v>
       </c>
       <c r="AF86" t="s" s="2">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="AG86" t="s" s="2">
         <v>80</v>
@@ -12632,10 +12635,10 @@
     </row>
     <row r="87" hidden="true">
       <c r="A87" t="s" s="2">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B87" t="s" s="2">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" t="s" s="2">
@@ -12658,13 +12661,13 @@
         <v>79</v>
       </c>
       <c r="K87" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="L87" t="s" s="2">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="M87" t="s" s="2">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="N87" s="2"/>
       <c r="O87" s="2"/>
@@ -12715,7 +12718,7 @@
         <v>79</v>
       </c>
       <c r="AF87" t="s" s="2">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="AG87" t="s" s="2">
         <v>80</v>
@@ -12733,7 +12736,7 @@
         <v>79</v>
       </c>
       <c r="AL87" t="s" s="2">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="AM87" t="s" s="2">
         <v>133</v>
@@ -12750,10 +12753,10 @@
     </row>
     <row r="88" hidden="true">
       <c r="A88" t="s" s="2">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B88" t="s" s="2">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" t="s" s="2">
@@ -12776,13 +12779,13 @@
         <v>79</v>
       </c>
       <c r="K88" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="L88" t="s" s="2">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="M88" t="s" s="2">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="N88" s="2"/>
       <c r="O88" s="2"/>
@@ -12833,7 +12836,7 @@
         <v>79</v>
       </c>
       <c r="AF88" t="s" s="2">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="AG88" t="s" s="2">
         <v>80</v>
@@ -12851,7 +12854,7 @@
         <v>79</v>
       </c>
       <c r="AL88" t="s" s="2">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="AM88" t="s" s="2">
         <v>133</v>
@@ -12868,10 +12871,10 @@
     </row>
     <row r="89" hidden="true">
       <c r="A89" t="s" s="2">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B89" t="s" s="2">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" t="s" s="2">
@@ -12897,10 +12900,10 @@
         <v>187</v>
       </c>
       <c r="L89" t="s" s="2">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="M89" t="s" s="2">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="N89" s="2"/>
       <c r="O89" s="2"/>
@@ -12927,13 +12930,13 @@
         <v>79</v>
       </c>
       <c r="X89" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Y89" t="s" s="2">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="Z89" t="s" s="2">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="AA89" t="s" s="2">
         <v>79</v>
@@ -12951,7 +12954,7 @@
         <v>79</v>
       </c>
       <c r="AF89" t="s" s="2">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="AG89" t="s" s="2">
         <v>80</v>
@@ -12969,7 +12972,7 @@
         <v>79</v>
       </c>
       <c r="AL89" t="s" s="2">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="AM89" t="s" s="2">
         <v>133</v>
@@ -12986,10 +12989,10 @@
     </row>
     <row r="90" hidden="true">
       <c r="A90" t="s" s="2">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B90" t="s" s="2">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" t="s" s="2">
@@ -13015,10 +13018,10 @@
         <v>187</v>
       </c>
       <c r="L90" t="s" s="2">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="M90" t="s" s="2">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="N90" s="2"/>
       <c r="O90" s="2"/>
@@ -13045,13 +13048,13 @@
         <v>79</v>
       </c>
       <c r="X90" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Y90" t="s" s="2">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="Z90" t="s" s="2">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="AA90" t="s" s="2">
         <v>79</v>
@@ -13069,7 +13072,7 @@
         <v>79</v>
       </c>
       <c r="AF90" t="s" s="2">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="AG90" t="s" s="2">
         <v>80</v>
@@ -13104,10 +13107,10 @@
     </row>
     <row r="91" hidden="true">
       <c r="A91" t="s" s="2">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B91" t="s" s="2">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" t="s" s="2">
@@ -13130,16 +13133,16 @@
         <v>79</v>
       </c>
       <c r="K91" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="L91" t="s" s="2">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="M91" t="s" s="2">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="N91" t="s" s="2">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="O91" s="2"/>
       <c r="P91" t="s" s="2">
@@ -13189,7 +13192,7 @@
         <v>79</v>
       </c>
       <c r="AF91" t="s" s="2">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="AG91" t="s" s="2">
         <v>80</v>
@@ -13207,10 +13210,10 @@
         <v>79</v>
       </c>
       <c r="AL91" t="s" s="2">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="AM91" t="s" s="2">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="AN91" t="s" s="2">
         <v>79</v>
@@ -13224,10 +13227,10 @@
     </row>
     <row r="92" hidden="true">
       <c r="A92" t="s" s="2">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B92" t="s" s="2">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" t="s" s="2">
@@ -13342,10 +13345,10 @@
     </row>
     <row r="93" hidden="true">
       <c r="A93" t="s" s="2">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B93" t="s" s="2">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" t="s" s="2">
@@ -13462,14 +13465,14 @@
     </row>
     <row r="94" hidden="true">
       <c r="A94" t="s" s="2">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B94" t="s" s="2">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="E94" s="2"/>
       <c r="F94" t="s" s="2">
@@ -13491,10 +13494,10 @@
         <v>136</v>
       </c>
       <c r="L94" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="M94" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="N94" t="s" s="2">
         <v>139</v>
@@ -13549,7 +13552,7 @@
         <v>79</v>
       </c>
       <c r="AF94" t="s" s="2">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="AG94" t="s" s="2">
         <v>80</v>
@@ -13584,10 +13587,10 @@
     </row>
     <row r="95" hidden="true">
       <c r="A95" t="s" s="2">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B95" t="s" s="2">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" t="s" s="2">
@@ -13610,13 +13613,13 @@
         <v>79</v>
       </c>
       <c r="K95" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="L95" t="s" s="2">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="M95" t="s" s="2">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="N95" s="2"/>
       <c r="O95" s="2"/>
@@ -13667,7 +13670,7 @@
         <v>79</v>
       </c>
       <c r="AF95" t="s" s="2">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="AG95" t="s" s="2">
         <v>80</v>
@@ -13685,10 +13688,10 @@
         <v>79</v>
       </c>
       <c r="AL95" t="s" s="2">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="AM95" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="AN95" t="s" s="2">
         <v>79</v>
@@ -13702,10 +13705,10 @@
     </row>
     <row r="96" hidden="true">
       <c r="A96" t="s" s="2">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="B96" t="s" s="2">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" t="s" s="2">
@@ -13728,13 +13731,13 @@
         <v>79</v>
       </c>
       <c r="K96" t="s" s="2">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="L96" t="s" s="2">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="M96" t="s" s="2">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="N96" s="2"/>
       <c r="O96" s="2"/>
@@ -13785,7 +13788,7 @@
         <v>79</v>
       </c>
       <c r="AF96" t="s" s="2">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="AG96" t="s" s="2">
         <v>80</v>
@@ -13803,10 +13806,10 @@
         <v>79</v>
       </c>
       <c r="AL96" t="s" s="2">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="AM96" t="s" s="2">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="AN96" t="s" s="2">
         <v>79</v>
@@ -13815,15 +13818,15 @@
         <v>79</v>
       </c>
       <c r="AP96" t="s" s="2">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row r="97" hidden="true">
       <c r="A97" t="s" s="2">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="B97" t="s" s="2">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="C97" s="2"/>
       <c r="D97" t="s" s="2">
@@ -13846,13 +13849,13 @@
         <v>79</v>
       </c>
       <c r="K97" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="L97" t="s" s="2">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="M97" t="s" s="2">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="N97" s="2"/>
       <c r="O97" s="2"/>
@@ -13903,7 +13906,7 @@
         <v>79</v>
       </c>
       <c r="AF97" t="s" s="2">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="AG97" t="s" s="2">
         <v>80</v>
@@ -13921,10 +13924,10 @@
         <v>79</v>
       </c>
       <c r="AL97" t="s" s="2">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="AM97" t="s" s="2">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="AN97" t="s" s="2">
         <v>79</v>
@@ -13938,10 +13941,10 @@
     </row>
     <row r="98" hidden="true">
       <c r="A98" t="s" s="2">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B98" t="s" s="2">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" t="s" s="2">
@@ -13964,13 +13967,13 @@
         <v>79</v>
       </c>
       <c r="K98" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="L98" t="s" s="2">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="M98" t="s" s="2">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="N98" s="2"/>
       <c r="O98" s="2"/>
@@ -14021,7 +14024,7 @@
         <v>79</v>
       </c>
       <c r="AF98" t="s" s="2">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="AG98" t="s" s="2">
         <v>80</v>
@@ -14056,10 +14059,10 @@
     </row>
     <row r="99" hidden="true">
       <c r="A99" t="s" s="2">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="B99" t="s" s="2">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" t="s" s="2">
@@ -14174,10 +14177,10 @@
     </row>
     <row r="100" hidden="true">
       <c r="A100" t="s" s="2">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="B100" t="s" s="2">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" t="s" s="2">
@@ -14294,14 +14297,14 @@
     </row>
     <row r="101" hidden="true">
       <c r="A101" t="s" s="2">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="B101" t="s" s="2">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="C101" s="2"/>
       <c r="D101" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="E101" s="2"/>
       <c r="F101" t="s" s="2">
@@ -14323,10 +14326,10 @@
         <v>136</v>
       </c>
       <c r="L101" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="M101" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="N101" t="s" s="2">
         <v>139</v>
@@ -14381,7 +14384,7 @@
         <v>79</v>
       </c>
       <c r="AF101" t="s" s="2">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="AG101" t="s" s="2">
         <v>80</v>
@@ -14416,10 +14419,10 @@
     </row>
     <row r="102" hidden="true">
       <c r="A102" t="s" s="2">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B102" t="s" s="2">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="C102" s="2"/>
       <c r="D102" t="s" s="2">
@@ -14445,10 +14448,10 @@
         <v>162</v>
       </c>
       <c r="L102" t="s" s="2">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="M102" t="s" s="2">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="N102" s="2"/>
       <c r="O102" s="2"/>
@@ -14499,7 +14502,7 @@
         <v>79</v>
       </c>
       <c r="AF102" t="s" s="2">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="AG102" t="s" s="2">
         <v>80</v>
@@ -14529,15 +14532,15 @@
         <v>79</v>
       </c>
       <c r="AP102" t="s" s="2">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="103" hidden="true">
       <c r="A103" t="s" s="2">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="B103" t="s" s="2">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="C103" s="2"/>
       <c r="D103" t="s" s="2">
@@ -14560,13 +14563,13 @@
         <v>79</v>
       </c>
       <c r="K103" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="L103" t="s" s="2">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="M103" t="s" s="2">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="N103" s="2"/>
       <c r="O103" s="2"/>
@@ -14617,7 +14620,7 @@
         <v>79</v>
       </c>
       <c r="AF103" t="s" s="2">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="AG103" t="s" s="2">
         <v>80</v>
@@ -14652,10 +14655,10 @@
     </row>
     <row r="104" hidden="true">
       <c r="A104" t="s" s="2">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="B104" t="s" s="2">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="C104" s="2"/>
       <c r="D104" t="s" s="2">
@@ -14681,10 +14684,10 @@
         <v>187</v>
       </c>
       <c r="L104" t="s" s="2">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="M104" t="s" s="2">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="N104" s="2"/>
       <c r="O104" s="2"/>
@@ -14711,13 +14714,13 @@
         <v>79</v>
       </c>
       <c r="X104" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Y104" t="s" s="2">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="Z104" t="s" s="2">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="AA104" t="s" s="2">
         <v>79</v>
@@ -14735,7 +14738,7 @@
         <v>79</v>
       </c>
       <c r="AF104" t="s" s="2">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="AG104" t="s" s="2">
         <v>80</v>
@@ -14770,10 +14773,10 @@
     </row>
     <row r="105" hidden="true">
       <c r="A105" t="s" s="2">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B105" t="s" s="2">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="C105" s="2"/>
       <c r="D105" t="s" s="2">
@@ -14796,16 +14799,16 @@
         <v>79</v>
       </c>
       <c r="K105" t="s" s="2">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="L105" t="s" s="2">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="M105" t="s" s="2">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="N105" t="s" s="2">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="O105" s="2"/>
       <c r="P105" t="s" s="2">
@@ -14855,7 +14858,7 @@
         <v>79</v>
       </c>
       <c r="AF105" t="s" s="2">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="AG105" t="s" s="2">
         <v>90</v>
@@ -14890,10 +14893,10 @@
     </row>
     <row r="106" hidden="true">
       <c r="A106" t="s" s="2">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="B106" t="s" s="2">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="C106" s="2"/>
       <c r="D106" t="s" s="2">
@@ -14916,16 +14919,16 @@
         <v>79</v>
       </c>
       <c r="K106" t="s" s="2">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="L106" t="s" s="2">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="M106" t="s" s="2">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="N106" t="s" s="2">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="O106" s="2"/>
       <c r="P106" t="s" s="2">
@@ -14975,7 +14978,7 @@
         <v>79</v>
       </c>
       <c r="AF106" t="s" s="2">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="AG106" t="s" s="2">
         <v>80</v>

</xml_diff>

<commit_message>
add API details for immunizations
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.immunization.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.immunization.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AP$104</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AP$105</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3955" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3993" uniqueCount="586">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-06-13T14:37:26-05:00</t>
+    <t>2023-06-13T16:30:05-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -84,32 +84,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>A profile on the Immunization that declares how MHV will expose PHR immunization.
-**Proposed mapping not yet approved for implementation**
-* Derived off of US-Core Immunization
-  * US-Core already requires: status, vaccineCode, patient, occurance[x], primarySource
-* must point at the patient
-* must have status of completed 
-* must have identifier as cross reference to original source
-* must have a code.text or code.coding from a valueset
-  * code.coding should be a CVX but we don't have such.
-  * Might have a CPT code
-* must have a date (occuranceDateTime) the vaccine was administered from the UI
-  * will also be used for recorded date
-* must be indicated this data are not official record (primarySource=false)
-* any reaction is recorded as a contained observation
-* may have a comment note
-* once created will have an id, versionId, lastUpdated.
-* Not sure if text will be populated
-Mapping from [ImmunizationTO](StructureDefinition-VA.MHV.PHR.immunization-mappings.html#mappings-for-vdif-to-mhv-phr-immunizationto)
-TODO Questions: 
-- The given mock example aligns with both VIA_v4.0.7_uat.wsdl and mockey-mdws3-service.wsdl. The VIA schema has more elements. The mapping is only for elements that were in both and for which I had an example. Better mapping can be done if specific schema can be identifed, and more rich mock example.
-- reaction appears to be a controlled vocabulary (e.g. FEVER), or is it a number (1-11 - convertReactionCode())?
-- contraindicated -- appears to be a number (e.g. 0). No idea what the values might be or what they might mean
-- id - presuming this is a persisted identifier we can cross-reference with
-- series - this appears to be a controlled vocabulary (e.g. COMPLETE). What are the possible values and what do they mean?
-- encounter - should we convert these to instances of FHIR Encounter?
-- could have function that converts a defined set of ImmunizationTO.name values to proper codes. This might be an advanced feature.</t>
+    <t>A profile on the Immunization that declares how MHV will expose PHR immunization.</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -969,9 +944,6 @@
   </si>
   <si>
     <t>FiveWs.context</t>
-  </si>
-  <si>
-    <t>GetEncounter(ImmunizationTO.encounter.[VisitTO])</t>
   </si>
   <si>
     <t>Immunization.occurrence[x]</t>
@@ -1431,7 +1403,7 @@
     <t>Immunization.performer.actor.display</t>
   </si>
   <si>
-    <t>GetPractitioner(ImmunizationTO.orderedBy.[UserTO])</t>
+    <t>GetPractitioner(ImmunizationTO.orderedBy.[UserTO]) | `OP`</t>
   </si>
   <si>
     <t>Immunization.note</t>
@@ -1791,9 +1763,6 @@
     <t>One possible path to achieve presumed immunity against a disease - within the context of an authority.</t>
   </si>
   <si>
-    <t>ImmunizationTO.series</t>
-  </si>
-  <si>
     <t>Immunization.protocolApplied.authority</t>
   </si>
   <si>
@@ -1832,6 +1801,19 @@
   </si>
   <si>
     <t>The use of an integer is preferred if known. A string should only be used in cases where an integer is not available (such as when documenting a recurring booster dose).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type:$this}
+</t>
+  </si>
+  <si>
+    <t>Immunization.protocolApplied.doseNumber[x]:doseNumberString</t>
+  </si>
+  <si>
+    <t>doseNumberString</t>
+  </si>
+  <si>
+    <t>ImmunizationTO.series</t>
   </si>
   <si>
     <t>Immunization.protocolApplied.seriesDoses[x]</t>
@@ -2168,7 +2150,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AP104"/>
+  <dimension ref="A1:AP105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -2177,9 +2159,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="45.24609375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="60.28125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="45.24609375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="5.2265625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="3" max="3" width="17.87109375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="6" max="6" width="2.15234375" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="2.15234375" customWidth="true" bestFit="true"/>
@@ -3318,7 +3300,7 @@
         <v>39</v>
       </c>
       <c r="H10" t="s" s="2">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="I10" t="s" s="2">
         <v>37</v>
@@ -6406,15 +6388,15 @@
         <v>37</v>
       </c>
       <c r="AP35" t="s" s="2">
-        <v>300</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -6437,16 +6419,16 @@
         <v>49</v>
       </c>
       <c r="K36" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="L36" t="s" s="2">
         <v>302</v>
       </c>
-      <c r="L36" t="s" s="2">
+      <c r="M36" t="s" s="2">
         <v>303</v>
       </c>
-      <c r="M36" t="s" s="2">
+      <c r="N36" t="s" s="2">
         <v>304</v>
-      </c>
-      <c r="N36" t="s" s="2">
-        <v>305</v>
       </c>
       <c r="O36" s="2"/>
       <c r="P36" t="s" s="2">
@@ -6496,7 +6478,7 @@
         <v>37</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>48</v>
@@ -6511,30 +6493,30 @@
         <v>60</v>
       </c>
       <c r="AK36" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="AL36" t="s" s="2">
         <v>306</v>
       </c>
-      <c r="AL36" t="s" s="2">
+      <c r="AM36" t="s" s="2">
         <v>307</v>
       </c>
-      <c r="AM36" t="s" s="2">
+      <c r="AN36" t="s" s="2">
         <v>308</v>
       </c>
-      <c r="AN36" t="s" s="2">
+      <c r="AO36" t="s" s="2">
         <v>309</v>
       </c>
-      <c r="AO36" t="s" s="2">
+      <c r="AP36" t="s" s="2">
         <v>310</v>
-      </c>
-      <c r="AP36" t="s" s="2">
-        <v>311</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -6548,7 +6530,7 @@
         <v>48</v>
       </c>
       <c r="H37" t="s" s="2">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="I37" t="s" s="2">
         <v>37</v>
@@ -6557,13 +6539,13 @@
         <v>37</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L37" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="M37" t="s" s="2">
         <v>313</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>314</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -6614,7 +6596,7 @@
         <v>37</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>38</v>
@@ -6635,24 +6617,24 @@
         <v>37</v>
       </c>
       <c r="AM37" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="AN37" t="s" s="2">
         <v>315</v>
       </c>
-      <c r="AN37" t="s" s="2">
-        <v>316</v>
-      </c>
       <c r="AO37" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AP37" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -6678,13 +6660,13 @@
         <v>265</v>
       </c>
       <c r="L38" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="M38" t="s" s="2">
         <v>318</v>
       </c>
-      <c r="M38" t="s" s="2">
+      <c r="N38" t="s" s="2">
         <v>319</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>320</v>
       </c>
       <c r="O38" s="2"/>
       <c r="P38" t="s" s="2">
@@ -6734,7 +6716,7 @@
         <v>37</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>38</v>
@@ -6752,27 +6734,27 @@
         <v>37</v>
       </c>
       <c r="AL38" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="AM38" t="s" s="2">
         <v>321</v>
       </c>
-      <c r="AM38" t="s" s="2">
+      <c r="AN38" t="s" s="2">
         <v>322</v>
       </c>
-      <c r="AN38" t="s" s="2">
+      <c r="AO38" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AP38" t="s" s="2">
         <v>323</v>
-      </c>
-      <c r="AO38" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AP38" t="s" s="2">
-        <v>324</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -6798,13 +6780,13 @@
         <v>145</v>
       </c>
       <c r="L39" t="s" s="2">
+        <v>325</v>
+      </c>
+      <c r="M39" t="s" s="2">
         <v>326</v>
       </c>
-      <c r="M39" t="s" s="2">
+      <c r="N39" t="s" s="2">
         <v>327</v>
-      </c>
-      <c r="N39" t="s" s="2">
-        <v>328</v>
       </c>
       <c r="O39" s="2"/>
       <c r="P39" t="s" s="2">
@@ -6833,11 +6815,11 @@
         <v>206</v>
       </c>
       <c r="Y39" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="Z39" t="s" s="2">
         <v>329</v>
       </c>
-      <c r="Z39" t="s" s="2">
-        <v>330</v>
-      </c>
       <c r="AA39" t="s" s="2">
         <v>37</v>
       </c>
@@ -6854,7 +6836,7 @@
         <v>37</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>38</v>
@@ -6872,13 +6854,13 @@
         <v>37</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AN39" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AO39" t="s" s="2">
         <v>37</v>
@@ -6889,10 +6871,10 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6903,7 +6885,7 @@
         <v>38</v>
       </c>
       <c r="G40" t="s" s="2">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="H40" t="s" s="2">
         <v>37</v>
@@ -6915,13 +6897,13 @@
         <v>37</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="L40" t="s" s="2">
         <v>333</v>
       </c>
-      <c r="L40" t="s" s="2">
+      <c r="M40" t="s" s="2">
         <v>334</v>
-      </c>
-      <c r="M40" t="s" s="2">
-        <v>335</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -6972,7 +6954,7 @@
         <v>37</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>38</v>
@@ -6984,19 +6966,19 @@
         <v>37</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="AK40" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="AL40" t="s" s="2">
         <v>336</v>
       </c>
-      <c r="AL40" t="s" s="2">
+      <c r="AM40" t="s" s="2">
         <v>337</v>
       </c>
-      <c r="AM40" t="s" s="2">
+      <c r="AN40" t="s" s="2">
         <v>338</v>
-      </c>
-      <c r="AN40" t="s" s="2">
-        <v>339</v>
       </c>
       <c r="AO40" t="s" s="2">
         <v>37</v>
@@ -7007,10 +6989,10 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -7125,10 +7107,10 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -7245,10 +7227,10 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -7274,13 +7256,13 @@
         <v>120</v>
       </c>
       <c r="L43" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="M43" t="s" s="2">
         <v>343</v>
       </c>
-      <c r="M43" t="s" s="2">
+      <c r="N43" t="s" s="2">
         <v>344</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>345</v>
       </c>
       <c r="O43" s="2"/>
       <c r="P43" t="s" s="2">
@@ -7330,16 +7312,16 @@
         <v>37</v>
       </c>
       <c r="AF43" t="s" s="2">
+        <v>345</v>
+      </c>
+      <c r="AG43" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AH43" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AI43" t="s" s="2">
         <v>346</v>
-      </c>
-      <c r="AG43" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AH43" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AI43" t="s" s="2">
-        <v>347</v>
       </c>
       <c r="AJ43" t="s" s="2">
         <v>60</v>
@@ -7365,10 +7347,10 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -7394,13 +7376,13 @@
         <v>62</v>
       </c>
       <c r="L44" t="s" s="2">
+        <v>348</v>
+      </c>
+      <c r="M44" t="s" s="2">
         <v>349</v>
       </c>
-      <c r="M44" t="s" s="2">
+      <c r="N44" t="s" s="2">
         <v>350</v>
-      </c>
-      <c r="N44" t="s" s="2">
-        <v>351</v>
       </c>
       <c r="O44" s="2"/>
       <c r="P44" t="s" s="2">
@@ -7429,28 +7411,28 @@
         <v>150</v>
       </c>
       <c r="Y44" t="s" s="2">
+        <v>351</v>
+      </c>
+      <c r="Z44" t="s" s="2">
         <v>352</v>
       </c>
-      <c r="Z44" t="s" s="2">
+      <c r="AA44" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB44" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC44" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD44" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE44" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AF44" t="s" s="2">
         <v>353</v>
-      </c>
-      <c r="AA44" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AB44" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AC44" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD44" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AE44" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AF44" t="s" s="2">
-        <v>354</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>38</v>
@@ -7485,10 +7467,10 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -7514,13 +7496,13 @@
         <v>106</v>
       </c>
       <c r="L45" t="s" s="2">
+        <v>355</v>
+      </c>
+      <c r="M45" t="s" s="2">
         <v>356</v>
       </c>
-      <c r="M45" t="s" s="2">
+      <c r="N45" t="s" s="2">
         <v>357</v>
-      </c>
-      <c r="N45" t="s" s="2">
-        <v>358</v>
       </c>
       <c r="O45" s="2"/>
       <c r="P45" t="s" s="2">
@@ -7570,7 +7552,7 @@
         <v>37</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>38</v>
@@ -7591,7 +7573,7 @@
         <v>37</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>37</v>
@@ -7605,10 +7587,10 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -7622,7 +7604,7 @@
         <v>48</v>
       </c>
       <c r="H46" t="s" s="2">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="I46" t="s" s="2">
         <v>37</v>
@@ -7634,13 +7616,13 @@
         <v>120</v>
       </c>
       <c r="L46" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="M46" t="s" s="2">
         <v>362</v>
       </c>
-      <c r="M46" t="s" s="2">
+      <c r="N46" t="s" s="2">
         <v>363</v>
-      </c>
-      <c r="N46" t="s" s="2">
-        <v>364</v>
       </c>
       <c r="O46" s="2"/>
       <c r="P46" t="s" s="2">
@@ -7690,7 +7672,7 @@
         <v>37</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>38</v>
@@ -7720,15 +7702,15 @@
         <v>37</v>
       </c>
       <c r="AP46" t="s" s="2">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -7739,10 +7721,10 @@
         <v>38</v>
       </c>
       <c r="G47" t="s" s="2">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="H47" t="s" s="2">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="I47" t="s" s="2">
         <v>37</v>
@@ -7754,10 +7736,10 @@
         <v>185</v>
       </c>
       <c r="L47" t="s" s="2">
+        <v>367</v>
+      </c>
+      <c r="M47" t="s" s="2">
         <v>368</v>
-      </c>
-      <c r="M47" t="s" s="2">
-        <v>369</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
@@ -7808,7 +7790,7 @@
         <v>37</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>38</v>
@@ -7826,27 +7808,27 @@
         <v>37</v>
       </c>
       <c r="AL47" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="AM47" t="s" s="2">
         <v>370</v>
       </c>
-      <c r="AM47" t="s" s="2">
+      <c r="AN47" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AO47" t="s" s="2">
         <v>371</v>
       </c>
-      <c r="AN47" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AO47" t="s" s="2">
+      <c r="AP47" t="s" s="2">
         <v>372</v>
-      </c>
-      <c r="AP47" t="s" s="2">
-        <v>373</v>
       </c>
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7857,10 +7839,10 @@
         <v>38</v>
       </c>
       <c r="G48" t="s" s="2">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="H48" t="s" s="2">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="I48" t="s" s="2">
         <v>37</v>
@@ -7872,10 +7854,10 @@
         <v>120</v>
       </c>
       <c r="L48" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="M48" t="s" s="2">
         <v>375</v>
-      </c>
-      <c r="M48" t="s" s="2">
-        <v>376</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
@@ -7926,7 +7908,7 @@
         <v>37</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>38</v>
@@ -7944,27 +7926,27 @@
         <v>37</v>
       </c>
       <c r="AL48" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="AM48" t="s" s="2">
         <v>377</v>
       </c>
-      <c r="AM48" t="s" s="2">
+      <c r="AN48" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AO48" t="s" s="2">
         <v>378</v>
       </c>
-      <c r="AN48" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AO48" t="s" s="2">
+      <c r="AP48" t="s" s="2">
         <v>379</v>
-      </c>
-      <c r="AP48" t="s" s="2">
-        <v>380</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7987,13 +7969,13 @@
         <v>37</v>
       </c>
       <c r="K49" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="L49" t="s" s="2">
         <v>382</v>
       </c>
-      <c r="L49" t="s" s="2">
+      <c r="M49" t="s" s="2">
         <v>383</v>
-      </c>
-      <c r="M49" t="s" s="2">
-        <v>384</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -8044,7 +8026,7 @@
         <v>37</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>38</v>
@@ -8062,10 +8044,10 @@
         <v>37</v>
       </c>
       <c r="AL49" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="AM49" t="s" s="2">
         <v>385</v>
-      </c>
-      <c r="AM49" t="s" s="2">
-        <v>386</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>37</v>
@@ -8079,10 +8061,10 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -8108,10 +8090,10 @@
         <v>145</v>
       </c>
       <c r="L50" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="M50" t="s" s="2">
         <v>388</v>
-      </c>
-      <c r="M50" t="s" s="2">
-        <v>389</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
@@ -8141,11 +8123,11 @@
         <v>206</v>
       </c>
       <c r="Y50" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="Z50" t="s" s="2">
         <v>390</v>
       </c>
-      <c r="Z50" t="s" s="2">
-        <v>391</v>
-      </c>
       <c r="AA50" t="s" s="2">
         <v>37</v>
       </c>
@@ -8162,7 +8144,7 @@
         <v>37</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>38</v>
@@ -8180,16 +8162,16 @@
         <v>37</v>
       </c>
       <c r="AL50" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="AM50" t="s" s="2">
         <v>392</v>
       </c>
-      <c r="AM50" t="s" s="2">
+      <c r="AN50" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AO50" t="s" s="2">
         <v>393</v>
-      </c>
-      <c r="AN50" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AO50" t="s" s="2">
-        <v>394</v>
       </c>
       <c r="AP50" t="s" s="2">
         <v>37</v>
@@ -8197,10 +8179,10 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -8315,10 +8297,10 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -8435,10 +8417,10 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -8557,10 +8539,10 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -8674,15 +8656,15 @@
         <v>37</v>
       </c>
       <c r="AP54" t="s" s="2">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
@@ -8708,10 +8690,10 @@
         <v>145</v>
       </c>
       <c r="L55" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="M55" t="s" s="2">
         <v>401</v>
-      </c>
-      <c r="M55" t="s" s="2">
-        <v>402</v>
       </c>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
@@ -8741,11 +8723,11 @@
         <v>206</v>
       </c>
       <c r="Y55" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="Z55" t="s" s="2">
         <v>403</v>
       </c>
-      <c r="Z55" t="s" s="2">
-        <v>404</v>
-      </c>
       <c r="AA55" t="s" s="2">
         <v>37</v>
       </c>
@@ -8762,7 +8744,7 @@
         <v>37</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>38</v>
@@ -8780,16 +8762,16 @@
         <v>37</v>
       </c>
       <c r="AL55" t="s" s="2">
+        <v>404</v>
+      </c>
+      <c r="AM55" t="s" s="2">
         <v>405</v>
       </c>
-      <c r="AM55" t="s" s="2">
+      <c r="AN55" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AO55" t="s" s="2">
         <v>406</v>
-      </c>
-      <c r="AN55" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AO55" t="s" s="2">
-        <v>407</v>
       </c>
       <c r="AP55" t="s" s="2">
         <v>37</v>
@@ -8797,10 +8779,10 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
@@ -8823,13 +8805,13 @@
         <v>37</v>
       </c>
       <c r="K56" t="s" s="2">
+        <v>408</v>
+      </c>
+      <c r="L56" t="s" s="2">
         <v>409</v>
       </c>
-      <c r="L56" t="s" s="2">
+      <c r="M56" t="s" s="2">
         <v>410</v>
-      </c>
-      <c r="M56" t="s" s="2">
-        <v>411</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
@@ -8880,7 +8862,7 @@
         <v>37</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>38</v>
@@ -8898,10 +8880,10 @@
         <v>37</v>
       </c>
       <c r="AL56" t="s" s="2">
+        <v>411</v>
+      </c>
+      <c r="AM56" t="s" s="2">
         <v>412</v>
-      </c>
-      <c r="AM56" t="s" s="2">
-        <v>413</v>
       </c>
       <c r="AN56" t="s" s="2">
         <v>37</v>
@@ -8915,10 +8897,10 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
@@ -8929,10 +8911,10 @@
         <v>38</v>
       </c>
       <c r="G57" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H57" t="s" s="2">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="I57" t="s" s="2">
         <v>37</v>
@@ -8941,13 +8923,13 @@
         <v>49</v>
       </c>
       <c r="K57" t="s" s="2">
+        <v>414</v>
+      </c>
+      <c r="L57" t="s" s="2">
         <v>415</v>
       </c>
-      <c r="L57" t="s" s="2">
+      <c r="M57" t="s" s="2">
         <v>416</v>
-      </c>
-      <c r="M57" t="s" s="2">
-        <v>417</v>
       </c>
       <c r="N57" s="2"/>
       <c r="O57" s="2"/>
@@ -8998,7 +8980,7 @@
         <v>37</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>38</v>
@@ -9013,13 +8995,13 @@
         <v>60</v>
       </c>
       <c r="AK57" t="s" s="2">
+        <v>417</v>
+      </c>
+      <c r="AL57" t="s" s="2">
         <v>418</v>
       </c>
-      <c r="AL57" t="s" s="2">
+      <c r="AM57" t="s" s="2">
         <v>419</v>
-      </c>
-      <c r="AM57" t="s" s="2">
-        <v>420</v>
       </c>
       <c r="AN57" t="s" s="2">
         <v>37</v>
@@ -9033,10 +9015,10 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
@@ -9151,10 +9133,10 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -9271,14 +9253,14 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" t="s" s="2">
@@ -9300,10 +9282,10 @@
         <v>94</v>
       </c>
       <c r="L60" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="M60" t="s" s="2">
         <v>425</v>
-      </c>
-      <c r="M60" t="s" s="2">
-        <v>426</v>
       </c>
       <c r="N60" t="s" s="2">
         <v>97</v>
@@ -9358,7 +9340,7 @@
         <v>37</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>38</v>
@@ -9393,10 +9375,10 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -9422,10 +9404,10 @@
         <v>145</v>
       </c>
       <c r="L61" t="s" s="2">
+        <v>428</v>
+      </c>
+      <c r="M61" t="s" s="2">
         <v>429</v>
-      </c>
-      <c r="M61" t="s" s="2">
-        <v>430</v>
       </c>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
@@ -9455,11 +9437,11 @@
         <v>150</v>
       </c>
       <c r="Y61" t="s" s="2">
+        <v>430</v>
+      </c>
+      <c r="Z61" t="s" s="2">
         <v>431</v>
       </c>
-      <c r="Z61" t="s" s="2">
-        <v>432</v>
-      </c>
       <c r="AA61" t="s" s="2">
         <v>37</v>
       </c>
@@ -9476,7 +9458,7 @@
         <v>37</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>38</v>
@@ -9491,13 +9473,13 @@
         <v>60</v>
       </c>
       <c r="AK61" t="s" s="2">
+        <v>432</v>
+      </c>
+      <c r="AL61" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AM61" t="s" s="2">
         <v>433</v>
-      </c>
-      <c r="AL61" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AM61" t="s" s="2">
-        <v>434</v>
       </c>
       <c r="AN61" t="s" s="2">
         <v>37</v>
@@ -9511,10 +9493,10 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
@@ -9537,16 +9519,16 @@
         <v>49</v>
       </c>
       <c r="K62" t="s" s="2">
+        <v>435</v>
+      </c>
+      <c r="L62" t="s" s="2">
         <v>436</v>
       </c>
-      <c r="L62" t="s" s="2">
+      <c r="M62" t="s" s="2">
         <v>437</v>
       </c>
-      <c r="M62" t="s" s="2">
+      <c r="N62" t="s" s="2">
         <v>438</v>
-      </c>
-      <c r="N62" t="s" s="2">
-        <v>439</v>
       </c>
       <c r="O62" s="2"/>
       <c r="P62" t="s" s="2">
@@ -9596,7 +9578,7 @@
         <v>37</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>48</v>
@@ -9611,16 +9593,16 @@
         <v>60</v>
       </c>
       <c r="AK62" t="s" s="2">
+        <v>439</v>
+      </c>
+      <c r="AL62" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AM62" t="s" s="2">
         <v>440</v>
       </c>
-      <c r="AL62" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AM62" t="s" s="2">
+      <c r="AN62" t="s" s="2">
         <v>441</v>
-      </c>
-      <c r="AN62" t="s" s="2">
-        <v>442</v>
       </c>
       <c r="AO62" t="s" s="2">
         <v>37</v>
@@ -9631,10 +9613,10 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
@@ -9749,10 +9731,10 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
@@ -9869,10 +9851,10 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" t="s" s="2">
@@ -9898,13 +9880,13 @@
         <v>120</v>
       </c>
       <c r="L65" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="M65" t="s" s="2">
         <v>343</v>
       </c>
-      <c r="M65" t="s" s="2">
+      <c r="N65" t="s" s="2">
         <v>344</v>
-      </c>
-      <c r="N65" t="s" s="2">
-        <v>345</v>
       </c>
       <c r="O65" s="2"/>
       <c r="P65" t="s" s="2">
@@ -9954,16 +9936,16 @@
         <v>37</v>
       </c>
       <c r="AF65" t="s" s="2">
+        <v>345</v>
+      </c>
+      <c r="AG65" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AH65" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AI65" t="s" s="2">
         <v>346</v>
-      </c>
-      <c r="AG65" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AH65" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AI65" t="s" s="2">
-        <v>347</v>
       </c>
       <c r="AJ65" t="s" s="2">
         <v>60</v>
@@ -9989,10 +9971,10 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
@@ -10018,13 +10000,13 @@
         <v>62</v>
       </c>
       <c r="L66" t="s" s="2">
+        <v>348</v>
+      </c>
+      <c r="M66" t="s" s="2">
         <v>349</v>
       </c>
-      <c r="M66" t="s" s="2">
+      <c r="N66" t="s" s="2">
         <v>350</v>
-      </c>
-      <c r="N66" t="s" s="2">
-        <v>351</v>
       </c>
       <c r="O66" s="2"/>
       <c r="P66" t="s" s="2">
@@ -10053,28 +10035,28 @@
         <v>150</v>
       </c>
       <c r="Y66" t="s" s="2">
+        <v>351</v>
+      </c>
+      <c r="Z66" t="s" s="2">
         <v>352</v>
       </c>
-      <c r="Z66" t="s" s="2">
+      <c r="AA66" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB66" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC66" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD66" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE66" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AF66" t="s" s="2">
         <v>353</v>
-      </c>
-      <c r="AA66" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AB66" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AC66" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD66" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AE66" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AF66" t="s" s="2">
-        <v>354</v>
       </c>
       <c r="AG66" t="s" s="2">
         <v>38</v>
@@ -10109,10 +10091,10 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" t="s" s="2">
@@ -10138,13 +10120,13 @@
         <v>106</v>
       </c>
       <c r="L67" t="s" s="2">
+        <v>355</v>
+      </c>
+      <c r="M67" t="s" s="2">
         <v>356</v>
       </c>
-      <c r="M67" t="s" s="2">
+      <c r="N67" t="s" s="2">
         <v>357</v>
-      </c>
-      <c r="N67" t="s" s="2">
-        <v>358</v>
       </c>
       <c r="O67" s="2"/>
       <c r="P67" t="s" s="2">
@@ -10194,7 +10176,7 @@
         <v>37</v>
       </c>
       <c r="AF67" t="s" s="2">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AG67" t="s" s="2">
         <v>38</v>
@@ -10215,7 +10197,7 @@
         <v>37</v>
       </c>
       <c r="AM67" t="s" s="2">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="AN67" t="s" s="2">
         <v>37</v>
@@ -10229,10 +10211,10 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B68" t="s" s="2">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" t="s" s="2">
@@ -10258,13 +10240,13 @@
         <v>120</v>
       </c>
       <c r="L68" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="M68" t="s" s="2">
         <v>362</v>
       </c>
-      <c r="M68" t="s" s="2">
+      <c r="N68" t="s" s="2">
         <v>363</v>
-      </c>
-      <c r="N68" t="s" s="2">
-        <v>364</v>
       </c>
       <c r="O68" s="2"/>
       <c r="P68" t="s" s="2">
@@ -10314,7 +10296,7 @@
         <v>37</v>
       </c>
       <c r="AF68" t="s" s="2">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AG68" t="s" s="2">
         <v>38</v>
@@ -10344,15 +10326,15 @@
         <v>37</v>
       </c>
       <c r="AP68" t="s" s="2">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B69" t="s" s="2">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" t="s" s="2">
@@ -10366,7 +10348,7 @@
         <v>48</v>
       </c>
       <c r="H69" t="s" s="2">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="I69" t="s" s="2">
         <v>37</v>
@@ -10375,13 +10357,13 @@
         <v>49</v>
       </c>
       <c r="K69" t="s" s="2">
+        <v>450</v>
+      </c>
+      <c r="L69" t="s" s="2">
         <v>451</v>
       </c>
-      <c r="L69" t="s" s="2">
+      <c r="M69" t="s" s="2">
         <v>452</v>
-      </c>
-      <c r="M69" t="s" s="2">
-        <v>453</v>
       </c>
       <c r="N69" s="2"/>
       <c r="O69" s="2"/>
@@ -10432,7 +10414,7 @@
         <v>37</v>
       </c>
       <c r="AF69" t="s" s="2">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="AG69" t="s" s="2">
         <v>38</v>
@@ -10447,13 +10429,13 @@
         <v>60</v>
       </c>
       <c r="AK69" t="s" s="2">
+        <v>453</v>
+      </c>
+      <c r="AL69" t="s" s="2">
         <v>454</v>
       </c>
-      <c r="AL69" t="s" s="2">
+      <c r="AM69" t="s" s="2">
         <v>455</v>
-      </c>
-      <c r="AM69" t="s" s="2">
-        <v>456</v>
       </c>
       <c r="AN69" t="s" s="2">
         <v>37</v>
@@ -10467,10 +10449,10 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" t="s" s="2">
@@ -10585,10 +10567,10 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" t="s" s="2">
@@ -10705,10 +10687,10 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" t="s" s="2">
@@ -10731,16 +10713,16 @@
         <v>49</v>
       </c>
       <c r="K72" t="s" s="2">
+        <v>459</v>
+      </c>
+      <c r="L72" t="s" s="2">
         <v>460</v>
       </c>
-      <c r="L72" t="s" s="2">
+      <c r="M72" t="s" s="2">
         <v>461</v>
       </c>
-      <c r="M72" t="s" s="2">
+      <c r="N72" t="s" s="2">
         <v>462</v>
-      </c>
-      <c r="N72" t="s" s="2">
-        <v>463</v>
       </c>
       <c r="O72" s="2"/>
       <c r="P72" t="s" s="2">
@@ -10790,7 +10772,7 @@
         <v>37</v>
       </c>
       <c r="AF72" t="s" s="2">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="AG72" t="s" s="2">
         <v>38</v>
@@ -10811,7 +10793,7 @@
         <v>91</v>
       </c>
       <c r="AM72" t="s" s="2">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AN72" t="s" s="2">
         <v>37</v>
@@ -10825,10 +10807,10 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" t="s" s="2">
@@ -10851,13 +10833,13 @@
         <v>49</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L73" t="s" s="2">
+        <v>466</v>
+      </c>
+      <c r="M73" t="s" s="2">
         <v>467</v>
-      </c>
-      <c r="M73" t="s" s="2">
-        <v>468</v>
       </c>
       <c r="N73" s="2"/>
       <c r="O73" s="2"/>
@@ -10908,7 +10890,7 @@
         <v>37</v>
       </c>
       <c r="AF73" t="s" s="2">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="AG73" t="s" s="2">
         <v>38</v>
@@ -10929,7 +10911,7 @@
         <v>91</v>
       </c>
       <c r="AM73" t="s" s="2">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="AN73" t="s" s="2">
         <v>37</v>
@@ -10943,10 +10925,10 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s" s="2">
@@ -10969,13 +10951,13 @@
         <v>49</v>
       </c>
       <c r="K74" t="s" s="2">
+        <v>471</v>
+      </c>
+      <c r="L74" t="s" s="2">
         <v>472</v>
       </c>
-      <c r="L74" t="s" s="2">
+      <c r="M74" t="s" s="2">
         <v>473</v>
-      </c>
-      <c r="M74" t="s" s="2">
-        <v>474</v>
       </c>
       <c r="N74" s="2"/>
       <c r="O74" s="2"/>
@@ -11026,7 +11008,7 @@
         <v>37</v>
       </c>
       <c r="AF74" t="s" s="2">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="AG74" t="s" s="2">
         <v>48</v>
@@ -11047,24 +11029,24 @@
         <v>91</v>
       </c>
       <c r="AM74" t="s" s="2">
+        <v>475</v>
+      </c>
+      <c r="AN74" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AO74" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AP74" t="s" s="2">
         <v>476</v>
-      </c>
-      <c r="AN74" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AO74" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AP74" t="s" s="2">
-        <v>477</v>
       </c>
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B75" t="s" s="2">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" t="s" s="2">
@@ -11090,10 +11072,10 @@
         <v>145</v>
       </c>
       <c r="L75" t="s" s="2">
+        <v>478</v>
+      </c>
+      <c r="M75" t="s" s="2">
         <v>479</v>
-      </c>
-      <c r="M75" t="s" s="2">
-        <v>480</v>
       </c>
       <c r="N75" s="2"/>
       <c r="O75" s="2"/>
@@ -11123,11 +11105,11 @@
         <v>206</v>
       </c>
       <c r="Y75" t="s" s="2">
+        <v>480</v>
+      </c>
+      <c r="Z75" t="s" s="2">
         <v>481</v>
       </c>
-      <c r="Z75" t="s" s="2">
-        <v>482</v>
-      </c>
       <c r="AA75" t="s" s="2">
         <v>37</v>
       </c>
@@ -11144,7 +11126,7 @@
         <v>37</v>
       </c>
       <c r="AF75" t="s" s="2">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AG75" t="s" s="2">
         <v>38</v>
@@ -11159,13 +11141,13 @@
         <v>60</v>
       </c>
       <c r="AK75" t="s" s="2">
+        <v>482</v>
+      </c>
+      <c r="AL75" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AM75" t="s" s="2">
         <v>483</v>
-      </c>
-      <c r="AL75" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AM75" t="s" s="2">
-        <v>484</v>
       </c>
       <c r="AN75" t="s" s="2">
         <v>37</v>
@@ -11179,10 +11161,10 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B76" t="s" s="2">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" t="s" s="2">
@@ -11205,13 +11187,13 @@
         <v>37</v>
       </c>
       <c r="K76" t="s" s="2">
+        <v>485</v>
+      </c>
+      <c r="L76" t="s" s="2">
+        <v>478</v>
+      </c>
+      <c r="M76" t="s" s="2">
         <v>486</v>
-      </c>
-      <c r="L76" t="s" s="2">
-        <v>479</v>
-      </c>
-      <c r="M76" t="s" s="2">
-        <v>487</v>
       </c>
       <c r="N76" s="2"/>
       <c r="O76" s="2"/>
@@ -11262,7 +11244,7 @@
         <v>37</v>
       </c>
       <c r="AF76" t="s" s="2">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="AG76" t="s" s="2">
         <v>38</v>
@@ -11277,7 +11259,7 @@
         <v>60</v>
       </c>
       <c r="AK76" t="s" s="2">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="AL76" t="s" s="2">
         <v>37</v>
@@ -11297,10 +11279,10 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B77" t="s" s="2">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" t="s" s="2">
@@ -11326,20 +11308,20 @@
         <v>265</v>
       </c>
       <c r="L77" t="s" s="2">
+        <v>489</v>
+      </c>
+      <c r="M77" t="s" s="2">
         <v>490</v>
       </c>
-      <c r="M77" t="s" s="2">
+      <c r="N77" t="s" s="2">
         <v>491</v>
-      </c>
-      <c r="N77" t="s" s="2">
-        <v>492</v>
       </c>
       <c r="O77" s="2"/>
       <c r="P77" t="s" s="2">
         <v>37</v>
       </c>
       <c r="Q77" t="s" s="2">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="R77" t="s" s="2">
         <v>37</v>
@@ -11384,7 +11366,7 @@
         <v>37</v>
       </c>
       <c r="AF77" t="s" s="2">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="AG77" t="s" s="2">
         <v>38</v>
@@ -11402,7 +11384,7 @@
         <v>37</v>
       </c>
       <c r="AL77" t="s" s="2">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="AM77" t="s" s="2">
         <v>91</v>
@@ -11419,10 +11401,10 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B78" t="s" s="2">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" t="s" s="2">
@@ -11448,10 +11430,10 @@
         <v>145</v>
       </c>
       <c r="L78" t="s" s="2">
+        <v>495</v>
+      </c>
+      <c r="M78" t="s" s="2">
         <v>496</v>
-      </c>
-      <c r="M78" t="s" s="2">
-        <v>497</v>
       </c>
       <c r="N78" s="2"/>
       <c r="O78" s="2"/>
@@ -11481,11 +11463,11 @@
         <v>206</v>
       </c>
       <c r="Y78" t="s" s="2">
+        <v>497</v>
+      </c>
+      <c r="Z78" t="s" s="2">
         <v>498</v>
       </c>
-      <c r="Z78" t="s" s="2">
-        <v>499</v>
-      </c>
       <c r="AA78" t="s" s="2">
         <v>37</v>
       </c>
@@ -11502,7 +11484,7 @@
         <v>37</v>
       </c>
       <c r="AF78" t="s" s="2">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="AG78" t="s" s="2">
         <v>38</v>
@@ -11537,10 +11519,10 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B79" t="s" s="2">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" t="s" s="2">
@@ -11563,13 +11545,13 @@
         <v>37</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="L79" t="s" s="2">
+        <v>500</v>
+      </c>
+      <c r="M79" t="s" s="2">
         <v>501</v>
-      </c>
-      <c r="M79" t="s" s="2">
-        <v>502</v>
       </c>
       <c r="N79" s="2"/>
       <c r="O79" s="2"/>
@@ -11620,7 +11602,7 @@
         <v>37</v>
       </c>
       <c r="AF79" t="s" s="2">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="AG79" t="s" s="2">
         <v>38</v>
@@ -11632,7 +11614,7 @@
         <v>37</v>
       </c>
       <c r="AJ79" t="s" s="2">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="AK79" t="s" s="2">
         <v>37</v>
@@ -11655,10 +11637,10 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B80" t="s" s="2">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" t="s" s="2">
@@ -11773,10 +11755,10 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B81" t="s" s="2">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" t="s" s="2">
@@ -11893,14 +11875,14 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B82" t="s" s="2">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" t="s" s="2">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E82" s="2"/>
       <c r="F82" t="s" s="2">
@@ -11922,10 +11904,10 @@
         <v>94</v>
       </c>
       <c r="L82" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="M82" t="s" s="2">
         <v>425</v>
-      </c>
-      <c r="M82" t="s" s="2">
-        <v>426</v>
       </c>
       <c r="N82" t="s" s="2">
         <v>97</v>
@@ -11980,7 +11962,7 @@
         <v>37</v>
       </c>
       <c r="AF82" t="s" s="2">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="AG82" t="s" s="2">
         <v>38</v>
@@ -12015,10 +11997,10 @@
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B83" t="s" s="2">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" t="s" s="2">
@@ -12044,10 +12026,10 @@
         <v>120</v>
       </c>
       <c r="L83" t="s" s="2">
+        <v>507</v>
+      </c>
+      <c r="M83" t="s" s="2">
         <v>508</v>
-      </c>
-      <c r="M83" t="s" s="2">
-        <v>509</v>
       </c>
       <c r="N83" s="2"/>
       <c r="O83" s="2"/>
@@ -12098,7 +12080,7 @@
         <v>37</v>
       </c>
       <c r="AF83" t="s" s="2">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="AG83" t="s" s="2">
         <v>38</v>
@@ -12116,7 +12098,7 @@
         <v>37</v>
       </c>
       <c r="AL83" t="s" s="2">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="AM83" t="s" s="2">
         <v>91</v>
@@ -12133,10 +12115,10 @@
     </row>
     <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B84" t="s" s="2">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" t="s" s="2">
@@ -12162,10 +12144,10 @@
         <v>62</v>
       </c>
       <c r="L84" t="s" s="2">
+        <v>511</v>
+      </c>
+      <c r="M84" t="s" s="2">
         <v>512</v>
-      </c>
-      <c r="M84" t="s" s="2">
-        <v>513</v>
       </c>
       <c r="N84" s="2"/>
       <c r="O84" s="2"/>
@@ -12216,7 +12198,7 @@
         <v>37</v>
       </c>
       <c r="AF84" t="s" s="2">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="AG84" t="s" s="2">
         <v>38</v>
@@ -12251,10 +12233,10 @@
     </row>
     <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B85" t="s" s="2">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" t="s" s="2">
@@ -12277,13 +12259,13 @@
         <v>37</v>
       </c>
       <c r="K85" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L85" t="s" s="2">
+        <v>514</v>
+      </c>
+      <c r="M85" t="s" s="2">
         <v>515</v>
-      </c>
-      <c r="M85" t="s" s="2">
-        <v>516</v>
       </c>
       <c r="N85" s="2"/>
       <c r="O85" s="2"/>
@@ -12334,7 +12316,7 @@
         <v>37</v>
       </c>
       <c r="AF85" t="s" s="2">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="AG85" t="s" s="2">
         <v>38</v>
@@ -12352,7 +12334,7 @@
         <v>37</v>
       </c>
       <c r="AL85" t="s" s="2">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="AM85" t="s" s="2">
         <v>91</v>
@@ -12369,10 +12351,10 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B86" t="s" s="2">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" t="s" s="2">
@@ -12395,13 +12377,13 @@
         <v>37</v>
       </c>
       <c r="K86" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L86" t="s" s="2">
+        <v>518</v>
+      </c>
+      <c r="M86" t="s" s="2">
         <v>519</v>
-      </c>
-      <c r="M86" t="s" s="2">
-        <v>520</v>
       </c>
       <c r="N86" s="2"/>
       <c r="O86" s="2"/>
@@ -12452,7 +12434,7 @@
         <v>37</v>
       </c>
       <c r="AF86" t="s" s="2">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AG86" t="s" s="2">
         <v>38</v>
@@ -12470,7 +12452,7 @@
         <v>37</v>
       </c>
       <c r="AL86" t="s" s="2">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="AM86" t="s" s="2">
         <v>91</v>
@@ -12487,10 +12469,10 @@
     </row>
     <row r="87" hidden="true">
       <c r="A87" t="s" s="2">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B87" t="s" s="2">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" t="s" s="2">
@@ -12516,10 +12498,10 @@
         <v>145</v>
       </c>
       <c r="L87" t="s" s="2">
+        <v>522</v>
+      </c>
+      <c r="M87" t="s" s="2">
         <v>523</v>
-      </c>
-      <c r="M87" t="s" s="2">
-        <v>524</v>
       </c>
       <c r="N87" s="2"/>
       <c r="O87" s="2"/>
@@ -12549,11 +12531,11 @@
         <v>206</v>
       </c>
       <c r="Y87" t="s" s="2">
+        <v>524</v>
+      </c>
+      <c r="Z87" t="s" s="2">
         <v>525</v>
       </c>
-      <c r="Z87" t="s" s="2">
-        <v>526</v>
-      </c>
       <c r="AA87" t="s" s="2">
         <v>37</v>
       </c>
@@ -12570,7 +12552,7 @@
         <v>37</v>
       </c>
       <c r="AF87" t="s" s="2">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="AG87" t="s" s="2">
         <v>38</v>
@@ -12588,7 +12570,7 @@
         <v>37</v>
       </c>
       <c r="AL87" t="s" s="2">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="AM87" t="s" s="2">
         <v>91</v>
@@ -12605,10 +12587,10 @@
     </row>
     <row r="88" hidden="true">
       <c r="A88" t="s" s="2">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B88" t="s" s="2">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" t="s" s="2">
@@ -12634,10 +12616,10 @@
         <v>145</v>
       </c>
       <c r="L88" t="s" s="2">
+        <v>528</v>
+      </c>
+      <c r="M88" t="s" s="2">
         <v>529</v>
-      </c>
-      <c r="M88" t="s" s="2">
-        <v>530</v>
       </c>
       <c r="N88" s="2"/>
       <c r="O88" s="2"/>
@@ -12667,11 +12649,11 @@
         <v>206</v>
       </c>
       <c r="Y88" t="s" s="2">
+        <v>530</v>
+      </c>
+      <c r="Z88" t="s" s="2">
         <v>531</v>
       </c>
-      <c r="Z88" t="s" s="2">
-        <v>532</v>
-      </c>
       <c r="AA88" t="s" s="2">
         <v>37</v>
       </c>
@@ -12688,7 +12670,7 @@
         <v>37</v>
       </c>
       <c r="AF88" t="s" s="2">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="AG88" t="s" s="2">
         <v>38</v>
@@ -12723,10 +12705,10 @@
     </row>
     <row r="89" hidden="true">
       <c r="A89" t="s" s="2">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B89" t="s" s="2">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" t="s" s="2">
@@ -12749,16 +12731,16 @@
         <v>37</v>
       </c>
       <c r="K89" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="L89" t="s" s="2">
+        <v>533</v>
+      </c>
+      <c r="M89" t="s" s="2">
         <v>534</v>
       </c>
-      <c r="M89" t="s" s="2">
+      <c r="N89" t="s" s="2">
         <v>535</v>
-      </c>
-      <c r="N89" t="s" s="2">
-        <v>536</v>
       </c>
       <c r="O89" s="2"/>
       <c r="P89" t="s" s="2">
@@ -12808,7 +12790,7 @@
         <v>37</v>
       </c>
       <c r="AF89" t="s" s="2">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="AG89" t="s" s="2">
         <v>38</v>
@@ -12826,10 +12808,10 @@
         <v>37</v>
       </c>
       <c r="AL89" t="s" s="2">
+        <v>536</v>
+      </c>
+      <c r="AM89" t="s" s="2">
         <v>537</v>
-      </c>
-      <c r="AM89" t="s" s="2">
-        <v>538</v>
       </c>
       <c r="AN89" t="s" s="2">
         <v>37</v>
@@ -12843,10 +12825,10 @@
     </row>
     <row r="90" hidden="true">
       <c r="A90" t="s" s="2">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B90" t="s" s="2">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" t="s" s="2">
@@ -12961,10 +12943,10 @@
     </row>
     <row r="91" hidden="true">
       <c r="A91" t="s" s="2">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B91" t="s" s="2">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" t="s" s="2">
@@ -13081,14 +13063,14 @@
     </row>
     <row r="92" hidden="true">
       <c r="A92" t="s" s="2">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B92" t="s" s="2">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" t="s" s="2">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E92" s="2"/>
       <c r="F92" t="s" s="2">
@@ -13110,10 +13092,10 @@
         <v>94</v>
       </c>
       <c r="L92" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="M92" t="s" s="2">
         <v>425</v>
-      </c>
-      <c r="M92" t="s" s="2">
-        <v>426</v>
       </c>
       <c r="N92" t="s" s="2">
         <v>97</v>
@@ -13168,7 +13150,7 @@
         <v>37</v>
       </c>
       <c r="AF92" t="s" s="2">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="AG92" t="s" s="2">
         <v>38</v>
@@ -13203,10 +13185,10 @@
     </row>
     <row r="93" hidden="true">
       <c r="A93" t="s" s="2">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B93" t="s" s="2">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" t="s" s="2">
@@ -13217,7 +13199,7 @@
         <v>38</v>
       </c>
       <c r="G93" t="s" s="2">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="H93" t="s" s="2">
         <v>37</v>
@@ -13229,13 +13211,13 @@
         <v>37</v>
       </c>
       <c r="K93" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L93" t="s" s="2">
+        <v>542</v>
+      </c>
+      <c r="M93" t="s" s="2">
         <v>543</v>
-      </c>
-      <c r="M93" t="s" s="2">
-        <v>544</v>
       </c>
       <c r="N93" s="2"/>
       <c r="O93" s="2"/>
@@ -13286,7 +13268,7 @@
         <v>37</v>
       </c>
       <c r="AF93" t="s" s="2">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AG93" t="s" s="2">
         <v>38</v>
@@ -13304,10 +13286,10 @@
         <v>37</v>
       </c>
       <c r="AL93" t="s" s="2">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="AM93" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AN93" t="s" s="2">
         <v>37</v>
@@ -13321,10 +13303,10 @@
     </row>
     <row r="94" hidden="true">
       <c r="A94" t="s" s="2">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B94" t="s" s="2">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" t="s" s="2">
@@ -13347,13 +13329,13 @@
         <v>37</v>
       </c>
       <c r="K94" t="s" s="2">
+        <v>546</v>
+      </c>
+      <c r="L94" t="s" s="2">
         <v>547</v>
       </c>
-      <c r="L94" t="s" s="2">
+      <c r="M94" t="s" s="2">
         <v>548</v>
-      </c>
-      <c r="M94" t="s" s="2">
-        <v>549</v>
       </c>
       <c r="N94" s="2"/>
       <c r="O94" s="2"/>
@@ -13404,7 +13386,7 @@
         <v>37</v>
       </c>
       <c r="AF94" t="s" s="2">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="AG94" t="s" s="2">
         <v>38</v>
@@ -13422,27 +13404,27 @@
         <v>37</v>
       </c>
       <c r="AL94" t="s" s="2">
+        <v>549</v>
+      </c>
+      <c r="AM94" t="s" s="2">
         <v>550</v>
       </c>
-      <c r="AM94" t="s" s="2">
+      <c r="AN94" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AO94" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AP94" t="s" s="2">
         <v>551</v>
-      </c>
-      <c r="AN94" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AO94" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AP94" t="s" s="2">
-        <v>552</v>
       </c>
     </row>
     <row r="95" hidden="true">
       <c r="A95" t="s" s="2">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B95" t="s" s="2">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" t="s" s="2">
@@ -13453,7 +13435,7 @@
         <v>38</v>
       </c>
       <c r="G95" t="s" s="2">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="H95" t="s" s="2">
         <v>37</v>
@@ -13468,10 +13450,10 @@
         <v>265</v>
       </c>
       <c r="L95" t="s" s="2">
+        <v>553</v>
+      </c>
+      <c r="M95" t="s" s="2">
         <v>554</v>
-      </c>
-      <c r="M95" t="s" s="2">
-        <v>555</v>
       </c>
       <c r="N95" s="2"/>
       <c r="O95" s="2"/>
@@ -13522,7 +13504,7 @@
         <v>37</v>
       </c>
       <c r="AF95" t="s" s="2">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="AG95" t="s" s="2">
         <v>38</v>
@@ -13540,10 +13522,10 @@
         <v>37</v>
       </c>
       <c r="AL95" t="s" s="2">
+        <v>555</v>
+      </c>
+      <c r="AM95" t="s" s="2">
         <v>556</v>
-      </c>
-      <c r="AM95" t="s" s="2">
-        <v>557</v>
       </c>
       <c r="AN95" t="s" s="2">
         <v>37</v>
@@ -13557,10 +13539,10 @@
     </row>
     <row r="96" hidden="true">
       <c r="A96" t="s" s="2">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B96" t="s" s="2">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" t="s" s="2">
@@ -13571,10 +13553,10 @@
         <v>38</v>
       </c>
       <c r="G96" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H96" t="s" s="2">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="I96" t="s" s="2">
         <v>37</v>
@@ -13583,13 +13565,13 @@
         <v>37</v>
       </c>
       <c r="K96" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="L96" t="s" s="2">
+        <v>558</v>
+      </c>
+      <c r="M96" t="s" s="2">
         <v>559</v>
-      </c>
-      <c r="M96" t="s" s="2">
-        <v>560</v>
       </c>
       <c r="N96" s="2"/>
       <c r="O96" s="2"/>
@@ -13640,7 +13622,7 @@
         <v>37</v>
       </c>
       <c r="AF96" t="s" s="2">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="AG96" t="s" s="2">
         <v>38</v>
@@ -13675,10 +13657,10 @@
     </row>
     <row r="97" hidden="true">
       <c r="A97" t="s" s="2">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B97" t="s" s="2">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C97" s="2"/>
       <c r="D97" t="s" s="2">
@@ -13793,10 +13775,10 @@
     </row>
     <row r="98" hidden="true">
       <c r="A98" t="s" s="2">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B98" t="s" s="2">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" t="s" s="2">
@@ -13913,14 +13895,14 @@
     </row>
     <row r="99" hidden="true">
       <c r="A99" t="s" s="2">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B99" t="s" s="2">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" t="s" s="2">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E99" s="2"/>
       <c r="F99" t="s" s="2">
@@ -13942,10 +13924,10 @@
         <v>94</v>
       </c>
       <c r="L99" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="M99" t="s" s="2">
         <v>425</v>
-      </c>
-      <c r="M99" t="s" s="2">
-        <v>426</v>
       </c>
       <c r="N99" t="s" s="2">
         <v>97</v>
@@ -14000,7 +13982,7 @@
         <v>37</v>
       </c>
       <c r="AF99" t="s" s="2">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="AG99" t="s" s="2">
         <v>38</v>
@@ -14035,10 +14017,10 @@
     </row>
     <row r="100" hidden="true">
       <c r="A100" t="s" s="2">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B100" t="s" s="2">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" t="s" s="2">
@@ -14049,7 +14031,7 @@
         <v>38</v>
       </c>
       <c r="G100" t="s" s="2">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="H100" t="s" s="2">
         <v>37</v>
@@ -14064,10 +14046,10 @@
         <v>120</v>
       </c>
       <c r="L100" t="s" s="2">
+        <v>564</v>
+      </c>
+      <c r="M100" t="s" s="2">
         <v>565</v>
-      </c>
-      <c r="M100" t="s" s="2">
-        <v>566</v>
       </c>
       <c r="N100" s="2"/>
       <c r="O100" s="2"/>
@@ -14118,7 +14100,7 @@
         <v>37</v>
       </c>
       <c r="AF100" t="s" s="2">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="AG100" t="s" s="2">
         <v>38</v>
@@ -14148,15 +14130,15 @@
         <v>37</v>
       </c>
       <c r="AP100" t="s" s="2">
-        <v>567</v>
+        <v>37</v>
       </c>
     </row>
     <row r="101" hidden="true">
       <c r="A101" t="s" s="2">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B101" t="s" s="2">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C101" s="2"/>
       <c r="D101" t="s" s="2">
@@ -14167,7 +14149,7 @@
         <v>38</v>
       </c>
       <c r="G101" t="s" s="2">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="H101" t="s" s="2">
         <v>37</v>
@@ -14182,10 +14164,10 @@
         <v>185</v>
       </c>
       <c r="L101" t="s" s="2">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="M101" t="s" s="2">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="N101" s="2"/>
       <c r="O101" s="2"/>
@@ -14236,7 +14218,7 @@
         <v>37</v>
       </c>
       <c r="AF101" t="s" s="2">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="AG101" t="s" s="2">
         <v>38</v>
@@ -14271,10 +14253,10 @@
     </row>
     <row r="102" hidden="true">
       <c r="A102" t="s" s="2">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B102" t="s" s="2">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C102" s="2"/>
       <c r="D102" t="s" s="2">
@@ -14285,7 +14267,7 @@
         <v>38</v>
       </c>
       <c r="G102" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H102" t="s" s="2">
         <v>37</v>
@@ -14300,10 +14282,10 @@
         <v>145</v>
       </c>
       <c r="L102" t="s" s="2">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="M102" t="s" s="2">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="N102" s="2"/>
       <c r="O102" s="2"/>
@@ -14333,10 +14315,10 @@
         <v>206</v>
       </c>
       <c r="Y102" t="s" s="2">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="Z102" t="s" s="2">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="AA102" t="s" s="2">
         <v>37</v>
@@ -14354,7 +14336,7 @@
         <v>37</v>
       </c>
       <c r="AF102" t="s" s="2">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="AG102" t="s" s="2">
         <v>38</v>
@@ -14389,10 +14371,10 @@
     </row>
     <row r="103" hidden="true">
       <c r="A103" t="s" s="2">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B103" t="s" s="2">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C103" s="2"/>
       <c r="D103" t="s" s="2">
@@ -14415,16 +14397,16 @@
         <v>37</v>
       </c>
       <c r="K103" t="s" s="2">
+        <v>575</v>
+      </c>
+      <c r="L103" t="s" s="2">
+        <v>576</v>
+      </c>
+      <c r="M103" t="s" s="2">
         <v>577</v>
       </c>
-      <c r="L103" t="s" s="2">
+      <c r="N103" t="s" s="2">
         <v>578</v>
-      </c>
-      <c r="M103" t="s" s="2">
-        <v>579</v>
-      </c>
-      <c r="N103" t="s" s="2">
-        <v>580</v>
       </c>
       <c r="O103" s="2"/>
       <c r="P103" t="s" s="2">
@@ -14462,19 +14444,17 @@
         <v>37</v>
       </c>
       <c r="AB103" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AC103" t="s" s="2">
-        <v>37</v>
-      </c>
+        <v>579</v>
+      </c>
+      <c r="AC103" s="2"/>
       <c r="AD103" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AE103" t="s" s="2">
-        <v>37</v>
+        <v>110</v>
       </c>
       <c r="AF103" t="s" s="2">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="AG103" t="s" s="2">
         <v>48</v>
@@ -14509,12 +14489,14 @@
     </row>
     <row r="104" hidden="true">
       <c r="A104" t="s" s="2">
+        <v>580</v>
+      </c>
+      <c r="B104" t="s" s="2">
+        <v>574</v>
+      </c>
+      <c r="C104" t="s" s="2">
         <v>581</v>
       </c>
-      <c r="B104" t="s" s="2">
-        <v>581</v>
-      </c>
-      <c r="C104" s="2"/>
       <c r="D104" t="s" s="2">
         <v>37</v>
       </c>
@@ -14526,7 +14508,7 @@
         <v>48</v>
       </c>
       <c r="H104" t="s" s="2">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="I104" t="s" s="2">
         <v>37</v>
@@ -14535,16 +14517,16 @@
         <v>37</v>
       </c>
       <c r="K104" t="s" s="2">
+        <v>120</v>
+      </c>
+      <c r="L104" t="s" s="2">
+        <v>576</v>
+      </c>
+      <c r="M104" t="s" s="2">
         <v>577</v>
       </c>
-      <c r="L104" t="s" s="2">
-        <v>582</v>
-      </c>
-      <c r="M104" t="s" s="2">
-        <v>583</v>
-      </c>
       <c r="N104" t="s" s="2">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="O104" s="2"/>
       <c r="P104" t="s" s="2">
@@ -14594,10 +14576,10 @@
         <v>37</v>
       </c>
       <c r="AF104" t="s" s="2">
-        <v>581</v>
+        <v>574</v>
       </c>
       <c r="AG104" t="s" s="2">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="AH104" t="s" s="2">
         <v>48</v>
@@ -14624,11 +14606,131 @@
         <v>37</v>
       </c>
       <c r="AP104" t="s" s="2">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="105" hidden="true">
+      <c r="A105" t="s" s="2">
+        <v>583</v>
+      </c>
+      <c r="B105" t="s" s="2">
+        <v>583</v>
+      </c>
+      <c r="C105" s="2"/>
+      <c r="D105" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="E105" s="2"/>
+      <c r="F105" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="G105" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="H105" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I105" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J105" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="K105" t="s" s="2">
+        <v>575</v>
+      </c>
+      <c r="L105" t="s" s="2">
+        <v>584</v>
+      </c>
+      <c r="M105" t="s" s="2">
+        <v>585</v>
+      </c>
+      <c r="N105" t="s" s="2">
+        <v>578</v>
+      </c>
+      <c r="O105" s="2"/>
+      <c r="P105" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Q105" s="2"/>
+      <c r="R105" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S105" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T105" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U105" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V105" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W105" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X105" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y105" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z105" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA105" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB105" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC105" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD105" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE105" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AF105" t="s" s="2">
+        <v>583</v>
+      </c>
+      <c r="AG105" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AH105" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AI105" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AJ105" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="AK105" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AL105" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AM105" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AN105" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AO105" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AP105" t="s" s="2">
         <v>37</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AP104">
+  <autoFilter ref="A1:AP105">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -14638,7 +14740,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI103">
+  <conditionalFormatting sqref="A2:AI104">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
update the API side documentation for allergy and immunization
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.immunization.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.immunization.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-08-18T06:56:10-05:00</t>
+    <t>2023-08-18T07:55:35-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1148,7 +1148,7 @@
     <t>Reference.display</t>
   </si>
   <si>
-    <t>GetLocation(ImmunizationTO.encounter.location.name)</t>
+    <t>ImmunizationTO.encounter.location.name</t>
   </si>
   <si>
     <t>Immunization.manufacturer</t>
@@ -6870,7 +6870,7 @@
         <v>48</v>
       </c>
       <c r="H40" t="s" s="2">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="I40" t="s" s="2">
         <v>37</v>
@@ -6948,7 +6948,7 @@
         <v>37</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="AK40" t="s" s="2">
         <v>335</v>
@@ -7586,7 +7586,7 @@
         <v>48</v>
       </c>
       <c r="H46" t="s" s="2">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="I46" t="s" s="2">
         <v>37</v>

</xml_diff>